<commit_message>
Added DS_ExcelData file, WaitUtils, JSUtils, LaunchPage, LoginPage, LinkedListPage, StackPage, StepDefinition files, TopicUrlRegistry files
Signed-off-by: SatyaJ <saphin.rao@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/DS_ExcelData.xlsx
+++ b/src/test/resources/DS_ExcelData.xlsx
@@ -1,27 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{2F4DB1E7-E69E-4E2B-B904-D09047465F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saphi\git\DS_Algo_Satya\src\test\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677BB2D0-E6C6-4A0D-804F-044620C56C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5745" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
   </bookViews>
   <sheets>
     <sheet name="StackPageContent" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginPageContent" sheetId="2" r:id="rId2"/>
+    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="79">
   <si>
     <t>scenario_type</t>
   </si>
@@ -84,14 +101,196 @@
   </si>
   <si>
     <t xml:space="preserve"> stack, pop or push</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>submission_method</t>
+  </si>
+  <si>
+    <t>Null value in cred</t>
+  </si>
+  <si>
+    <t>submits the login form</t>
+  </si>
+  <si>
+    <t>Please fill out this field.</t>
+  </si>
+  <si>
+    <t>presses Enter</t>
+  </si>
+  <si>
+    <t>Null value in password</t>
+  </si>
+  <si>
+    <t>validUser</t>
+  </si>
+  <si>
+    <t>Null value in username</t>
+  </si>
+  <si>
+    <t>validPass</t>
+  </si>
+  <si>
+    <t>Invalid cred</t>
+  </si>
+  <si>
+    <t>typoUser</t>
+  </si>
+  <si>
+    <t>initiates login</t>
+  </si>
+  <si>
+    <t>Invalid username and password</t>
+  </si>
+  <si>
+    <t>confirms login using Enter</t>
+  </si>
+  <si>
+    <t>Invalid password</t>
+  </si>
+  <si>
+    <t>typoPass</t>
+  </si>
+  <si>
+    <t>valid_login</t>
+  </si>
+  <si>
+    <t>Submits the login form</t>
+  </si>
+  <si>
+    <t>You are logged in</t>
+  </si>
+  <si>
+    <t>expected_message</t>
+  </si>
+  <si>
+    <t>code_snippet</t>
+  </si>
+  <si>
+    <t>expected_output</t>
+  </si>
+  <si>
+    <t>error_message</t>
+  </si>
+  <si>
+    <t>print(Hello)</t>
+  </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <t>SyntaxError</t>
+  </si>
+  <si>
+    <t>Traversal</t>
+  </si>
+  <si>
+    <t>NameError</t>
+  </si>
+  <si>
+    <t>Deletion</t>
+  </si>
+  <si>
+    <t>print(10+15))</t>
+  </si>
+  <si>
+    <t>Creating Linked List</t>
+  </si>
+  <si>
+    <t>Implement Linked List in Python</t>
+  </si>
+  <si>
+    <t>Insertion</t>
+  </si>
+  <si>
+    <t>print('Hello Introduction')</t>
+  </si>
+  <si>
+    <t>Hello Introduction</t>
+  </si>
+  <si>
+    <t>print('Hello Creating Linked List')</t>
+  </si>
+  <si>
+    <t>Hello Creating Linked List</t>
+  </si>
+  <si>
+    <t>print('Hello Types of Linked List')</t>
+  </si>
+  <si>
+    <t>print('Hello Implement Linked List in python')</t>
+  </si>
+  <si>
+    <t>Hello Implement Linked List in python</t>
+  </si>
+  <si>
+    <t>print('Hello Traversal')</t>
+  </si>
+  <si>
+    <t>Hello Traversal</t>
+  </si>
+  <si>
+    <t>print('Hello Insertion')</t>
+  </si>
+  <si>
+    <t>Hello Insertion</t>
+  </si>
+  <si>
+    <t>print('Hello Deletion')</t>
+  </si>
+  <si>
+    <t>Hello Deletion</t>
+  </si>
+  <si>
+    <t>Types of Linked List</t>
+  </si>
+  <si>
+    <t>Hello Types of Linked List</t>
+  </si>
+  <si>
+    <t>print(5+3)</t>
+  </si>
+  <si>
+    <t>print('Stack Implementation')</t>
+  </si>
+  <si>
+    <t>Stack Implementation</t>
+  </si>
+  <si>
+    <t>print(Stack.pop())</t>
+  </si>
+  <si>
+    <t>Stack Operations</t>
+  </si>
+  <si>
+    <t>print('Stack Applications')</t>
+  </si>
+  <si>
+    <t>print('Stack Applications'))</t>
+  </si>
+  <si>
+    <t>print('Stack Operations')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -119,8 +318,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C00EDDC-8DF7-469B-AF31-0E608F45A4C6}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -468,10 +673,13 @@
     <col min="3" max="3" width="18.86328125" customWidth="1"/>
     <col min="4" max="4" width="23.06640625" customWidth="1"/>
     <col min="5" max="5" width="17.19921875" customWidth="1"/>
-    <col min="6" max="6" width="28.6640625" customWidth="1"/>
+    <col min="6" max="6" width="43.73046875" customWidth="1"/>
+    <col min="7" max="7" width="23.796875" customWidth="1"/>
+    <col min="8" max="8" width="19.19921875" customWidth="1"/>
+    <col min="9" max="9" width="15.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -490,8 +698,17 @@
       <c r="F1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -499,7 +716,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -507,7 +724,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -518,7 +735,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -529,7 +746,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -540,7 +757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -551,7 +768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -562,7 +779,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -571,6 +788,499 @@
       </c>
       <c r="F9" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" t="s">
+        <v>71</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" t="s">
+        <v>76</v>
+      </c>
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E22CFC9-75A9-4703-AAF7-30F647CF300B}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20.1328125" customWidth="1"/>
+    <col min="2" max="2" width="17.06640625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="22.9296875" customWidth="1"/>
+    <col min="5" max="5" width="17.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="57" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE905CA-1CE9-466F-88A4-C019229BCBBF}">
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection sqref="A1:D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.06640625" customWidth="1"/>
+    <col min="2" max="2" width="24.265625" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Launch and login feature reviewed and fixed
</commit_message>
<xml_diff>
--- a/src/test/resources/DS_ExcelData.xlsx
+++ b/src/test/resources/DS_ExcelData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saphi\git\DS_Algo_Satya\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cfb26f557d7176db/Desktop/DsalgoTeams/DS_Algo/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677BB2D0-E6C6-4A0D-804F-044620C56C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{677BB2D0-E6C6-4A0D-804F-044620C56C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84466E09-2975-44C1-BB08-913BED05F065}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
   </bookViews>
   <sheets>
     <sheet name="StackPageContent" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
   <si>
     <t>scenario_type</t>
   </si>
@@ -121,9 +121,6 @@
     <t>Please fill out this field.</t>
   </si>
   <si>
-    <t>presses Enter</t>
-  </si>
-  <si>
     <t>Null value in password</t>
   </si>
   <si>
@@ -136,21 +133,12 @@
     <t>validPass</t>
   </si>
   <si>
-    <t>Invalid cred</t>
-  </si>
-  <si>
     <t>typoUser</t>
   </si>
   <si>
     <t>initiates login</t>
   </si>
   <si>
-    <t>Invalid username and password</t>
-  </si>
-  <si>
-    <t>confirms login using Enter</t>
-  </si>
-  <si>
     <t>Invalid password</t>
   </si>
   <si>
@@ -275,6 +263,12 @@
   </si>
   <si>
     <t>print('Stack Operations')</t>
+  </si>
+  <si>
+    <t>Invalid  user</t>
+  </si>
+  <si>
+    <t>Invalid Username and Password</t>
   </si>
 </sst>
 </file>
@@ -341,6 +335,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -666,20 +664,20 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.9296875" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" customWidth="1"/>
-    <col min="3" max="3" width="18.86328125" customWidth="1"/>
-    <col min="4" max="4" width="23.06640625" customWidth="1"/>
-    <col min="5" max="5" width="17.19921875" customWidth="1"/>
-    <col min="6" max="6" width="43.73046875" customWidth="1"/>
-    <col min="7" max="7" width="23.796875" customWidth="1"/>
-    <col min="8" max="8" width="19.19921875" customWidth="1"/>
-    <col min="9" max="9" width="15.46484375" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -699,16 +697,16 @@
         <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -716,7 +714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -724,7 +722,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -735,7 +733,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -746,7 +744,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -757,7 +755,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -768,7 +766,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -779,7 +777,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -790,70 +788,70 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="I12" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="H13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="H14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -863,20 +861,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E22CFC9-75A9-4703-AAF7-30F647CF300B}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.1328125" customWidth="1"/>
-    <col min="2" max="2" width="17.06640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="22.9296875" customWidth="1"/>
-    <col min="5" max="5" width="17.265625" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -890,10 +890,10 @@
         <v>23</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -906,27 +906,29 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>25</v>
       </c>
@@ -934,155 +936,60 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="D7" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1090,197 +997,197 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE905CA-1CE9-466F-88A4-C019229BCBBF}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection sqref="A1:D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.06640625" customWidth="1"/>
-    <col min="2" max="2" width="24.265625" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>47</v>
-      </c>
       <c r="B2" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Graph try editor excel reader added
</commit_message>
<xml_diff>
--- a/src/test/resources/DS_ExcelData.xlsx
+++ b/src/test/resources/DS_ExcelData.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saphi\git\DS_Algo_Satya\src\test\resources\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677BB2D0-E6C6-4A0D-804F-044620C56C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" activeTab="2" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15156" windowHeight="2328" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="StackPageContent" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginPageContent" sheetId="2" r:id="rId2"/>
-    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId3"/>
+    <sheet name="GraphPageContent" sheetId="4" r:id="rId2"/>
+    <sheet name="LoginPageContent" sheetId="2" r:id="rId3"/>
+    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:G6"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="87">
   <si>
     <t>scenario_type</t>
   </si>
@@ -275,13 +271,37 @@
   </si>
   <si>
     <t>print('Stack Operations')</t>
+  </si>
+  <si>
+    <t>code_type</t>
+  </si>
+  <si>
+    <t>expected_result</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>an error popup stating NameError: name 'invalid' is not defined on line1</t>
+  </si>
+  <si>
+    <t>Graph Representations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,27 +679,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C00EDDC-8DF7-469B-AF31-0E608F45A4C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="13.9296875" customWidth="1"/>
+    <col min="1" max="1" width="13.8984375" customWidth="1"/>
     <col min="2" max="2" width="14.3984375" customWidth="1"/>
-    <col min="3" max="3" width="18.86328125" customWidth="1"/>
-    <col min="4" max="4" width="23.06640625" customWidth="1"/>
+    <col min="3" max="3" width="18.8984375" customWidth="1"/>
+    <col min="4" max="4" width="23.09765625" customWidth="1"/>
     <col min="5" max="5" width="17.19921875" customWidth="1"/>
-    <col min="6" max="6" width="43.73046875" customWidth="1"/>
+    <col min="6" max="6" width="43.69921875" customWidth="1"/>
     <col min="7" max="7" width="23.796875" customWidth="1"/>
     <col min="8" max="8" width="19.19921875" customWidth="1"/>
-    <col min="9" max="9" width="15.46484375" customWidth="1"/>
+    <col min="9" max="9" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -708,7 +728,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -716,7 +736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -724,7 +744,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -735,7 +755,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -746,7 +766,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -757,7 +777,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -768,7 +788,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -779,7 +799,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -790,7 +810,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -801,7 +821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -812,7 +832,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -823,7 +843,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -834,7 +854,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -845,7 +865,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -862,223 +882,73 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E22CFC9-75A9-4703-AAF7-30F647CF300B}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="20.1328125" customWidth="1"/>
-    <col min="2" max="2" width="17.06640625" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
-    <col min="4" max="4" width="22.9296875" customWidth="1"/>
-    <col min="5" max="5" width="17.265625" customWidth="1"/>
+    <col min="1" max="1" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="57" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>41</v>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1087,22 +957,247 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE905CA-1CE9-466F-88A4-C019229BCBBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView topLeftCell="A11" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="20.09765625" customWidth="1"/>
+    <col min="2" max="2" width="17.09765625" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="22.8984375" customWidth="1"/>
+    <col min="5" max="5" width="17.296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="27.6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="27.6">
+      <c r="A2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="27.6">
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="27.6">
+      <c r="A4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="27.6">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="27.6">
+      <c r="A6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="27.6">
+      <c r="A7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="27.6">
+      <c r="A8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="27.6">
+      <c r="A9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="27.6">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="27.6">
+      <c r="A11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection sqref="A1:D15"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C9" sqref="C6:C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="18.06640625" customWidth="1"/>
-    <col min="2" max="2" width="24.265625" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.09765625" customWidth="1"/>
+    <col min="2" max="2" width="24.296875" customWidth="1"/>
+    <col min="3" max="3" width="20.296875" customWidth="1"/>
     <col min="4" max="4" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1116,7 +1211,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
@@ -1128,7 +1223,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="43.2" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>47</v>
       </c>
@@ -1140,7 +1235,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="43.2" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -1152,7 +1247,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="43.2" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>53</v>
       </c>
@@ -1164,7 +1259,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="43.2" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>69</v>
       </c>
@@ -1176,7 +1271,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="43.2" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>69</v>
       </c>
@@ -1188,7 +1283,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="43.2" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
@@ -1200,7 +1295,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="43.2" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>54</v>
       </c>
@@ -1212,7 +1307,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" ht="43.2" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>49</v>
       </c>
@@ -1224,7 +1319,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="32.700000000000003" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
@@ -1236,7 +1331,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="32.700000000000003" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>55</v>
       </c>
@@ -1248,7 +1343,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="32.700000000000003" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>55</v>
       </c>
@@ -1260,7 +1355,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="32.700000000000003" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>51</v>
       </c>
@@ -1272,7 +1367,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>51</v>
       </c>

</xml_diff>

<commit_message>
updating excel with reshma modules
</commit_message>
<xml_diff>
--- a/src/test/resources/DS_ExcelData.xlsx
+++ b/src/test/resources/DS_ExcelData.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cfb26f557d7176db/Desktop/DsalgoTeams/DS_Algo/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rresh\eclipse-workspace\DSAlgo_Automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{677BB2D0-E6C6-4A0D-804F-044620C56C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84466E09-2975-44C1-BB08-913BED05F065}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{875D538C-C833-43CC-ABBA-18DFD8A76E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
   </bookViews>
   <sheets>
     <sheet name="StackPageContent" sheetId="1" r:id="rId1"/>
     <sheet name="LoginPageContent" sheetId="2" r:id="rId2"/>
-    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId3"/>
+    <sheet name="RegisterPage_labels" sheetId="4" r:id="rId3"/>
+    <sheet name="RegisterPage_Negativetestdata" sheetId="5" r:id="rId4"/>
+    <sheet name="RegisterPage_Validdata" sheetId="6" r:id="rId5"/>
+    <sheet name="QueueEditor" sheetId="7" r:id="rId6"/>
+    <sheet name="TreePage_topics" sheetId="8" r:id="rId7"/>
+    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="163">
   <si>
     <t>scenario_type</t>
   </si>
@@ -269,13 +274,274 @@
   </si>
   <si>
     <t>Invalid Username and Password</t>
+  </si>
+  <si>
+    <t>expected_result</t>
+  </si>
+  <si>
+    <t>Validate labels text in Register UI</t>
+  </si>
+  <si>
+    <t>Username:</t>
+  </si>
+  <si>
+    <t>Password:</t>
+  </si>
+  <si>
+    <t>Password confirmation:</t>
+  </si>
+  <si>
+    <t>Validate links text in Register UI</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Sign in</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Company name must be present in nav bar</t>
+  </si>
+  <si>
+    <t>NumpyNinja</t>
+  </si>
+  <si>
+    <t>password entry rules</t>
+  </si>
+  <si>
+    <t>Your password can’t be too similar to your other personal information.</t>
+  </si>
+  <si>
+    <t>Your password must contain at least 8 characters.</t>
+  </si>
+  <si>
+    <t>Your password can’t be a commonly used password.</t>
+  </si>
+  <si>
+    <t>Your password can’t be entirely numeric.</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>without username</t>
+  </si>
+  <si>
+    <t>Qaninja@123</t>
+  </si>
+  <si>
+    <t>without password</t>
+  </si>
+  <si>
+    <t>qatest</t>
+  </si>
+  <si>
+    <t>without confirm password</t>
+  </si>
+  <si>
+    <t>with specialcharacter password</t>
+  </si>
+  <si>
+    <t>testdata3</t>
+  </si>
+  <si>
+    <t>"@@@</t>
+  </si>
+  <si>
+    <t>Password does not match requirement</t>
+  </si>
+  <si>
+    <t>with password less then eight characters</t>
+  </si>
+  <si>
+    <t>A!1</t>
+  </si>
+  <si>
+    <t>with mismatch password</t>
+  </si>
+  <si>
+    <t>qatest123</t>
+  </si>
+  <si>
+    <t>Qaninja@1</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>with specialcharacter username</t>
+  </si>
+  <si>
+    <t>!@!</t>
+  </si>
+  <si>
+    <t>Username must be alphanumeric</t>
+  </si>
+  <si>
+    <t>valid register</t>
+  </si>
+  <si>
+    <t>Validrun01</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>Implementation of Queue in Python</t>
+  </si>
+  <si>
+    <t>print('hello')</t>
+  </si>
+  <si>
+    <t>hello</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>NameError: name 'abcd' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>Implementation using collections.deque</t>
+  </si>
+  <si>
+    <t>print(2+5.0)</t>
+  </si>
+  <si>
+    <t>print('a)</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>Implementation using array</t>
+  </si>
+  <si>
+    <t>print('abcd')</t>
+  </si>
+  <si>
+    <t>prin('hi')</t>
+  </si>
+  <si>
+    <t>NameError: name 'prin' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>Queue Operations</t>
+  </si>
+  <si>
+    <t>print('Queue')</t>
+  </si>
+  <si>
+    <t>Queue</t>
+  </si>
+  <si>
+    <t>print(5/0)</t>
+  </si>
+  <si>
+    <t>ZeroDivisionError: integer division or modulo by zero on line 1</t>
+  </si>
+  <si>
+    <t>expected_subtopic</t>
+  </si>
+  <si>
+    <t>Tree subtopic</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Overview of Trees </t>
+  </si>
+  <si>
+    <t>overview-of-trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminologies </t>
+  </si>
+  <si>
+    <t>terminologies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Types of Trees </t>
+  </si>
+  <si>
+    <t>types-of-trees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tree Traversals </t>
+  </si>
+  <si>
+    <t>tree-traversals</t>
+  </si>
+  <si>
+    <t>Traversals-Illustration</t>
+  </si>
+  <si>
+    <t>traversals-illustration</t>
+  </si>
+  <si>
+    <t>Binary Trees</t>
+  </si>
+  <si>
+    <t>binary-trees</t>
+  </si>
+  <si>
+    <t>Types of Binary Trees</t>
+  </si>
+  <si>
+    <t>types-of-binary-trees</t>
+  </si>
+  <si>
+    <t>Implementation in Python</t>
+  </si>
+  <si>
+    <t>implementation-in-python</t>
+  </si>
+  <si>
+    <t>Binary Tree Traversals</t>
+  </si>
+  <si>
+    <t>binary-tree-traversals</t>
+  </si>
+  <si>
+    <t>Implementation of Binary Trees</t>
+  </si>
+  <si>
+    <t>implementation-of-binary-trees</t>
+  </si>
+  <si>
+    <t>Applications of Binary trees</t>
+  </si>
+  <si>
+    <t>applications-of-binary-trees</t>
+  </si>
+  <si>
+    <t>Binary Search Trees</t>
+  </si>
+  <si>
+    <t>binary-search-trees</t>
+  </si>
+  <si>
+    <t>Implementation Of BST</t>
+  </si>
+  <si>
+    <t>implementation-of-bst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,6 +556,26 @@
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -309,10 +595,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -320,8 +607,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -335,10 +636,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -660,24 +957,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C00EDDC-8DF7-469B-AF31-0E608F45A4C6}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="18.86328125" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="43.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="6" width="43.73046875" customWidth="1"/>
+    <col min="7" max="7" width="23.86328125" customWidth="1"/>
+    <col min="8" max="8" width="19.1328125" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +1003,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -714,7 +1011,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -722,7 +1019,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -733,7 +1030,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -744,7 +1041,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -755,7 +1052,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -766,7 +1063,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -777,7 +1074,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -788,7 +1085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -799,7 +1096,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -810,7 +1107,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -821,7 +1118,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -832,7 +1129,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -843,7 +1140,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -863,20 +1160,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E22CFC9-75A9-4703-AAF7-30F647CF300B}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.1328125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.73046875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,7 +1190,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -906,7 +1203,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -921,7 +1218,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -936,7 +1233,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
@@ -953,7 +1250,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -970,7 +1267,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -994,6 +1291,648 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51C5CAA3-FB1D-4BCE-9182-B2FA9F84C576}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="36.1328125" customWidth="1"/>
+    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020B9FD9-2E14-4CAF-A8E0-943A614CB909}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="22.19921875" customWidth="1"/>
+    <col min="2" max="2" width="20.19921875" customWidth="1"/>
+    <col min="3" max="3" width="15.265625" customWidth="1"/>
+    <col min="4" max="4" width="14.06640625" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>101</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B8" t="s">
+        <v>110</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C6" r:id="rId1" display="A@1" xr:uid="{2582E95A-A213-42CD-B586-3A4F4C1B19E0}"/>
+    <hyperlink ref="C7" r:id="rId2" xr:uid="{29524C1E-6076-47C7-B805-6D76D374D347}"/>
+    <hyperlink ref="D7" r:id="rId3" xr:uid="{FF387820-06D8-496F-81AC-EF4D0A05F1D8}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{58EB9D2D-A0EA-4DC5-8F73-B51775CF3BEB}"/>
+    <hyperlink ref="C4" r:id="rId5" xr:uid="{2BF38257-934E-43DE-A016-3DDAA7F77291}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BC9BE92-D62F-45FA-91E2-BECBAFCCDAB7}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="18.06640625" customWidth="1"/>
+    <col min="2" max="2" width="16.73046875" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="17.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8137DEB-2A21-4D51-A3CA-F107661E405D}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.86328125" customWidth="1"/>
+    <col min="2" max="2" width="21.59765625" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="26.46484375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D4" s="6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A8" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="A9" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E2F82-668C-443C-A67D-2A4602EECA4D}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="20.1328125" customWidth="1"/>
+    <col min="2" max="2" width="34.53125" customWidth="1"/>
+    <col min="3" max="3" width="27.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>136</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="C7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="C13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>136</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE905CA-1CE9-466F-88A4-C019229BCBBF}">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -1001,15 +1940,15 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.265625" customWidth="1"/>
+    <col min="3" max="3" width="20.265625" customWidth="1"/>
+    <col min="4" max="4" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1962,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -1035,7 +1974,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -1047,7 +1986,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1059,7 +1998,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -1071,7 +2010,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>65</v>
       </c>
@@ -1083,7 +2022,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>65</v>
       </c>
@@ -1095,7 +2034,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
         <v>50</v>
       </c>
@@ -1107,7 +2046,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1119,7 +2058,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1131,7 +2070,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -1143,7 +2082,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1155,7 +2094,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1167,7 +2106,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -1179,7 +2118,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Review completed for Register Module
</commit_message>
<xml_diff>
--- a/src/test/resources/DS_ExcelData.xlsx
+++ b/src/test/resources/DS_ExcelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rresh\eclipse-workspace\DSAlgo_Automation\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cfb26f557d7176db/Desktop/DsalgoTeams/DS_Algo/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E38D46D1-35C2-43E0-A62F-F004006E5A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" firstSheet="4" activeTab="5" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
+    <workbookView xWindow="6195" yWindow="5955" windowWidth="21600" windowHeight="11175" tabRatio="868" activeTab="3" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
   </bookViews>
   <sheets>
     <sheet name="StackPageContent" sheetId="1" r:id="rId1"/>
@@ -968,20 +968,20 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.3984375" customWidth="1"/>
-    <col min="3" max="3" width="18.86328125" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="17.1328125" customWidth="1"/>
-    <col min="6" max="6" width="43.73046875" customWidth="1"/>
-    <col min="7" max="7" width="23.86328125" customWidth="1"/>
-    <col min="8" max="8" width="19.1328125" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" customWidth="1"/>
+    <col min="6" max="6" width="43.7109375" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1048,7 +1048,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1059,7 +1059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1070,7 +1070,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -1081,7 +1081,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -1092,7 +1092,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1136,7 +1136,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1147,7 +1147,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -1171,16 +1171,16 @@
       <selection sqref="A1:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.1328125" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="25.73046875" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1197,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -1210,7 +1210,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -1225,7 +1225,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -1240,7 +1240,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -1305,13 +1305,13 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.1328125" customWidth="1"/>
-    <col min="2" max="2" width="56.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.140625" customWidth="1"/>
+    <col min="2" max="2" width="56.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -1327,7 +1327,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>78</v>
       </c>
@@ -1335,7 +1335,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>78</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -1360,21 +1360,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020B9FD9-2E14-4CAF-A8E0-943A614CB909}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="20.19921875" customWidth="1"/>
-    <col min="3" max="3" width="15.265625" customWidth="1"/>
-    <col min="4" max="4" width="14.06640625" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="26" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.3984375" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>137</v>
       </c>
@@ -1412,7 +1412,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>138</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>85</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>89</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>91</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -1526,7 +1526,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>139</v>
       </c>
@@ -1546,10 +1546,10 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
   </sheetData>
@@ -1573,14 +1573,14 @@
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.59765625" customWidth="1"/>
+    <col min="1" max="2" width="21.5703125" customWidth="1"/>
     <col min="3" max="3" width="29" customWidth="1"/>
-    <col min="4" max="4" width="26.46484375" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>143</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>144</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>145</v>
       </c>
@@ -1636,7 +1636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>146</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>147</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>148</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>149</v>
       </c>
@@ -1692,7 +1692,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>150</v>
       </c>
@@ -1715,17 +1715,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF6E2F82-668C-443C-A67D-2A4602EECA4D}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.53125" customWidth="1"/>
-    <col min="2" max="2" width="27.19921875" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="2" max="2" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>112</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>116</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>118</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>120</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>122</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>124</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>126</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>128</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>130</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>132</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>134</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>136</v>
       </c>
@@ -1850,15 +1850,15 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="24.265625" customWidth="1"/>
-    <col min="3" max="3" width="20.265625" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -1884,7 +1884,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1908,7 +1908,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>65</v>
       </c>
@@ -1932,7 +1932,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>65</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>50</v>
       </c>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1980,7 +1980,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -1992,7 +1992,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -2016,7 +2016,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Login, Launch , Register - Completed
</commit_message>
<xml_diff>
--- a/src/test/resources/DS_ExcelData.xlsx
+++ b/src/test/resources/DS_ExcelData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cfb26f557d7176db/Desktop/DsalgoTeams/DS_Algo/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{677BB2D0-E6C6-4A0D-804F-044620C56C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84466E09-2975-44C1-BB08-913BED05F065}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{677BB2D0-E6C6-4A0D-804F-044620C56C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10C6D6B0-2F04-4F0E-BEB3-C932A36ABC29}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
+    <workbookView xWindow="6195" yWindow="4305" windowWidth="21600" windowHeight="11175" activeTab="1" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
   </bookViews>
   <sheets>
     <sheet name="StackPageContent" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginPageContent" sheetId="2" r:id="rId2"/>
-    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId3"/>
+    <sheet name="RegisterPage_Validdata" sheetId="4" r:id="rId2"/>
+    <sheet name="LoginPageContent" sheetId="2" r:id="rId3"/>
+    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="100">
   <si>
     <t>scenario_type</t>
   </si>
@@ -269,6 +270,75 @@
   </si>
   <si>
     <t>Invalid Username and Password</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>Qaninja@123</t>
+  </si>
+  <si>
+    <t>submits the register form</t>
+  </si>
+  <si>
+    <t>qatest</t>
+  </si>
+  <si>
+    <t>testdata3</t>
+  </si>
+  <si>
+    <t>@@@	@@@</t>
+  </si>
+  <si>
+    <t>Password does not match requirement</t>
+  </si>
+  <si>
+    <t>A!1</t>
+  </si>
+  <si>
+    <t>qatest123</t>
+  </si>
+  <si>
+    <t>Qaninja@1</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>!@!</t>
+  </si>
+  <si>
+    <t>Username must be alphanumeric</t>
+  </si>
+  <si>
+    <t>valid_register</t>
+  </si>
+  <si>
+    <t>Validrun04</t>
+  </si>
+  <si>
+    <t>New Account Created. You are logged in as username</t>
+  </si>
+  <si>
+    <t>Null value in password for register</t>
+  </si>
+  <si>
+    <t>Null value in  username for register</t>
+  </si>
+  <si>
+    <t>Null value in  confirm password for register</t>
+  </si>
+  <si>
+    <t>with specialcharacter password for register</t>
+  </si>
+  <si>
+    <t>with password less then eight characters for register</t>
+  </si>
+  <si>
+    <t>with mismatch password for register</t>
+  </si>
+  <si>
+    <t>with specialcharacter username for register</t>
   </si>
 </sst>
 </file>
@@ -312,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -320,6 +390,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -660,7 +731,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C00EDDC-8DF7-469B-AF31-0E608F45A4C6}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -860,10 +931,201 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8E81C6-F1AD-4746-9FF7-E156CBEBDFA4}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.85546875" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E22CFC9-75A9-4703-AAF7-30F647CF300B}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -993,7 +1255,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE905CA-1CE9-466F-88A4-C019229BCBBF}">
   <dimension ref="A1:D15"/>
   <sheetViews>

</xml_diff>

<commit_message>
pushed code to avoid conflicts before pulling new master
</commit_message>
<xml_diff>
--- a/src/test/resources/DS_ExcelData.xlsx
+++ b/src/test/resources/DS_ExcelData.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cfb26f557d7176db/Desktop/DsalgoTeams/DS_Algo/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{677BB2D0-E6C6-4A0D-804F-044620C56C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84466E09-2975-44C1-BB08-913BED05F065}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15156" windowHeight="9912" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="StackPageContent" sheetId="1" r:id="rId1"/>
     <sheet name="LoginPageContent" sheetId="2" r:id="rId2"/>
-    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId3"/>
+    <sheet name="GraphPageContent" sheetId="4" r:id="rId3"/>
+    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:L26"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="85">
   <si>
     <t>scenario_type</t>
   </si>
@@ -269,13 +265,66 @@
   </si>
   <si>
     <t>Invalid Username and Password</t>
+  </si>
+  <si>
+    <t>code_type</t>
+  </si>
+  <si>
+    <t>expected_result</t>
+  </si>
+  <si>
+    <t>Graph</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>Graph Representations</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">an error popup stating NameError: name </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'invalid'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is not defined on line </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF008000"/>
+        <rFont val="Aptos Narrow"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +338,18 @@
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF008000"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -312,7 +373,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -320,6 +381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -335,10 +397,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -657,27 +715,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C00EDDC-8DF7-469B-AF31-0E608F45A4C6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.3984375" customWidth="1"/>
+    <col min="3" max="3" width="18.8984375" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="43.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.09765625" customWidth="1"/>
+    <col min="6" max="6" width="43.69921875" customWidth="1"/>
+    <col min="7" max="7" width="23.8984375" customWidth="1"/>
+    <col min="8" max="8" width="19.09765625" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -706,7 +764,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -714,7 +772,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -722,7 +780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -733,7 +791,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -744,7 +802,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -755,7 +813,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -766,7 +824,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -777,7 +835,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
         <v>14</v>
       </c>
@@ -788,7 +846,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -799,7 +857,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -810,7 +868,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -821,7 +879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -832,7 +890,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -843,7 +901,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -860,23 +918,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E22CFC9-75A9-4703-AAF7-30F647CF300B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.09765625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.69921875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,7 +951,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="30">
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
@@ -906,7 +964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="30">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -921,7 +979,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="30">
       <c r="A4" s="2" t="s">
         <v>29</v>
       </c>
@@ -936,7 +994,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="30">
       <c r="A5" s="2" t="s">
         <v>75</v>
       </c>
@@ -953,7 +1011,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="30">
       <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
@@ -970,7 +1028,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -994,22 +1052,97 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE905CA-1CE9-466F-88A4-C019229BCBBF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="1" max="1" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.59765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.296875" customWidth="1"/>
+    <col min="3" max="3" width="20.296875" customWidth="1"/>
+    <col min="4" max="4" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1023,7 +1156,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -1035,7 +1168,7 @@
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="43.2" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>43</v>
       </c>
@@ -1047,7 +1180,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.2" customHeight="1">
       <c r="A4" s="2" t="s">
         <v>49</v>
       </c>
@@ -1059,7 +1192,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.2" customHeight="1">
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
@@ -1071,7 +1204,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="43.2" customHeight="1">
       <c r="A6" s="2" t="s">
         <v>65</v>
       </c>
@@ -1083,7 +1216,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="43.2" customHeight="1">
       <c r="A7" s="2" t="s">
         <v>65</v>
       </c>
@@ -1095,7 +1228,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="43.2" customHeight="1">
       <c r="A8" s="2" t="s">
         <v>50</v>
       </c>
@@ -1107,7 +1240,7 @@
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="43.2" customHeight="1">
       <c r="A9" s="2" t="s">
         <v>50</v>
       </c>
@@ -1119,7 +1252,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="43.2" customHeight="1">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1131,7 +1264,7 @@
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="32.700000000000003" customHeight="1">
       <c r="A11" s="2" t="s">
         <v>45</v>
       </c>
@@ -1143,7 +1276,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="32.700000000000003" customHeight="1">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1155,7 +1288,7 @@
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="32.700000000000003" customHeight="1">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
@@ -1167,7 +1300,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="32.700000000000003" customHeight="1">
       <c r="A14" s="2" t="s">
         <v>47</v>
       </c>
@@ -1179,7 +1312,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Added LinkedList module and Stack module
Signed-off-by: SatyaJ <saphin.rao@gmail.com>
</commit_message>
<xml_diff>
--- a/src/test/resources/DS_ExcelData.xlsx
+++ b/src/test/resources/DS_ExcelData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cfb26f557d7176db/Desktop/DsalgoTeams/DS_Algo/src/test/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saphi\git\DS_Algo_Satya\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="13_ncr:1_{677BB2D0-E6C6-4A0D-804F-044620C56C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{62B84646-6794-40B0-AE13-08F50641561C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF5E9CB-BEDF-4E97-93F0-CBC200DFE613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6195" yWindow="4305" windowWidth="21600" windowHeight="11175" activeTab="2" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
+    <workbookView xWindow="5745" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
   </bookViews>
   <sheets>
     <sheet name="StackPageContent" sheetId="1" r:id="rId1"/>
@@ -40,69 +40,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="87">
   <si>
     <t>scenario_type</t>
   </si>
   <si>
-    <t>static_content</t>
-  </si>
-  <si>
-    <t>expected_text</t>
-  </si>
-  <si>
-    <t>Stack</t>
-  </si>
-  <si>
-    <t>Topics Covered</t>
-  </si>
-  <si>
-    <t>topic_navigation</t>
-  </si>
-  <si>
-    <t>topic</t>
-  </si>
-  <si>
-    <t>page_url</t>
-  </si>
-  <si>
-    <t>Implementation</t>
-  </si>
-  <si>
     <t>Applications</t>
   </si>
   <si>
-    <t>/stack/operations-in-stack/</t>
-  </si>
-  <si>
-    <t>/stack/implementation</t>
-  </si>
-  <si>
-    <t>/stack/stack-applications</t>
-  </si>
-  <si>
     <t>Operations in Stack</t>
   </si>
   <si>
-    <t>scroll_validation</t>
-  </si>
-  <si>
-    <t>topic_page</t>
-  </si>
-  <si>
-    <t>expected_content</t>
-  </si>
-  <si>
     <t>Stack Applications</t>
-  </si>
-  <si>
-    <t>push, pop, overflow, underflow</t>
-  </si>
-  <si>
-    <t>Reverse Order, Undo, Call Stack, Parentheses Balance</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> stack, pop or push</t>
   </si>
   <si>
     <t>username</t>
@@ -357,6 +306,9 @@
 arr = [12, 23, 45, 67, 6, 90]
 # Test case 1
 search(arr, 12) </t>
+  </si>
+  <si>
+    <t>Implementation</t>
   </si>
 </sst>
 </file>
@@ -746,200 +698,109 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C00EDDC-8DF7-469B-AF31-0E608F45A4C6}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="43.7109375" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.140625" customWidth="1"/>
-    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="23.53125" customWidth="1"/>
+    <col min="4" max="4" width="26.59765625" customWidth="1"/>
+    <col min="5" max="5" width="17.1328125" customWidth="1"/>
+    <col min="6" max="6" width="43.73046875" customWidth="1"/>
+    <col min="7" max="7" width="23.86328125" customWidth="1"/>
+    <col min="8" max="8" width="19.1328125" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" t="s">
-        <v>40</v>
-      </c>
-      <c r="I1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="G10" t="s">
-        <v>67</v>
-      </c>
-      <c r="H10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" t="s">
-        <v>68</v>
-      </c>
-      <c r="H11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="G12" t="s">
-        <v>70</v>
-      </c>
-      <c r="I12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="G13" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" t="s">
-        <v>72</v>
-      </c>
-      <c r="H14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" t="s">
-        <v>73</v>
-      </c>
-      <c r="I15" t="s">
-        <v>44</v>
+      <c r="B7" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -953,182 +814,182 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="37.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.59765625" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.73046875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.86328125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>94</v>
-      </c>
       <c r="C2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="B5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="B6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="B7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>99</v>
-      </c>
       <c r="B8" s="3" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1140,28 +1001,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE007A3-BDC4-4CCF-89DD-DFF030394921}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="165" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1177,124 +1038,124 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.1328125" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.73046875" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1311,193 +1172,193 @@
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="24.265625" customWidth="1"/>
+    <col min="3" max="3" width="20.265625" customWidth="1"/>
+    <col min="4" max="4" width="19.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="2" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected few lines and changed pom.xml
</commit_message>
<xml_diff>
--- a/src/test/resources/DS_ExcelData.xlsx
+++ b/src/test/resources/DS_ExcelData.xlsx
@@ -5,19 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saphi\git\DS_Algo_Satya\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saphi\git\DS_Algo\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF5E9CB-BEDF-4E97-93F0-CBC200DFE613}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B1B89B-4A59-41EB-9142-528EDCCA8CB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5745" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
+    <workbookView xWindow="5745" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B73CB05F-107B-41ED-85A9-C212C46F3310}"/>
   </bookViews>
   <sheets>
-    <sheet name="StackPageContent" sheetId="1" r:id="rId1"/>
-    <sheet name="RegisterPage_Validdata" sheetId="4" r:id="rId2"/>
-    <sheet name="ArrayQuestion" sheetId="5" r:id="rId3"/>
-    <sheet name="LoginPageContent" sheetId="2" r:id="rId4"/>
-    <sheet name="LinkedListPageContent" sheetId="3" r:id="rId5"/>
+    <sheet name="RegisterPage_Validdata" sheetId="4" r:id="rId1"/>
+    <sheet name="ArrayQuestion" sheetId="5" r:id="rId2"/>
+    <sheet name="LoginPageContent" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,20 +38,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>scenario_type</t>
   </si>
   <si>
-    <t>Applications</t>
-  </si>
-  <si>
-    <t>Operations in Stack</t>
-  </si>
-  <si>
-    <t>Stack Applications</t>
-  </si>
-  <si>
     <t>username</t>
   </si>
   <si>
@@ -106,114 +95,6 @@
   </si>
   <si>
     <t>expected_message</t>
-  </si>
-  <si>
-    <t>code_snippet</t>
-  </si>
-  <si>
-    <t>expected_output</t>
-  </si>
-  <si>
-    <t>error_message</t>
-  </si>
-  <si>
-    <t>print(Hello)</t>
-  </si>
-  <si>
-    <t>Introduction</t>
-  </si>
-  <si>
-    <t>SyntaxError</t>
-  </si>
-  <si>
-    <t>Traversal</t>
-  </si>
-  <si>
-    <t>NameError</t>
-  </si>
-  <si>
-    <t>Deletion</t>
-  </si>
-  <si>
-    <t>print(10+15))</t>
-  </si>
-  <si>
-    <t>Creating Linked List</t>
-  </si>
-  <si>
-    <t>Implement Linked List in Python</t>
-  </si>
-  <si>
-    <t>Insertion</t>
-  </si>
-  <si>
-    <t>print('Hello Introduction')</t>
-  </si>
-  <si>
-    <t>Hello Introduction</t>
-  </si>
-  <si>
-    <t>print('Hello Creating Linked List')</t>
-  </si>
-  <si>
-    <t>Hello Creating Linked List</t>
-  </si>
-  <si>
-    <t>print('Hello Types of Linked List')</t>
-  </si>
-  <si>
-    <t>print('Hello Implement Linked List in python')</t>
-  </si>
-  <si>
-    <t>Hello Implement Linked List in python</t>
-  </si>
-  <si>
-    <t>print('Hello Traversal')</t>
-  </si>
-  <si>
-    <t>Hello Traversal</t>
-  </si>
-  <si>
-    <t>print('Hello Insertion')</t>
-  </si>
-  <si>
-    <t>Hello Insertion</t>
-  </si>
-  <si>
-    <t>print('Hello Deletion')</t>
-  </si>
-  <si>
-    <t>Hello Deletion</t>
-  </si>
-  <si>
-    <t>Types of Linked List</t>
-  </si>
-  <si>
-    <t>Hello Types of Linked List</t>
-  </si>
-  <si>
-    <t>print(5+3)</t>
-  </si>
-  <si>
-    <t>print('Stack Implementation')</t>
-  </si>
-  <si>
-    <t>Stack Implementation</t>
-  </si>
-  <si>
-    <t>print(Stack.pop())</t>
-  </si>
-  <si>
-    <t>Stack Operations</t>
-  </si>
-  <si>
-    <t>print('Stack Applications')</t>
-  </si>
-  <si>
-    <t>print('Stack Applications'))</t>
-  </si>
-  <si>
-    <t>print('Stack Operations')</t>
   </si>
   <si>
     <t>Invalid  user</t>
@@ -306,9 +187,6 @@
 arr = [12, 23, 45, 67, 6, 90]
 # Test case 1
 search(arr, 12) </t>
-  </si>
-  <si>
-    <t>Implementation</t>
   </si>
 </sst>
 </file>
@@ -697,118 +575,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C00EDDC-8DF7-469B-AF31-0E608F45A4C6}">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.53125" customWidth="1"/>
-    <col min="4" max="4" width="26.59765625" customWidth="1"/>
-    <col min="5" max="5" width="17.1328125" customWidth="1"/>
-    <col min="6" max="6" width="43.73046875" customWidth="1"/>
-    <col min="7" max="7" width="23.86328125" customWidth="1"/>
-    <col min="8" max="8" width="19.1328125" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="2">
-        <v>8</v>
-      </c>
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D5" s="2"/>
-    </row>
-    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A8E81C6-F1AD-4746-9FF7-E156CBEBDFA4}">
   <dimension ref="A1:F9"/>
   <sheetViews>
@@ -829,167 +595,167 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" s="3" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="3" t="s">
-        <v>76</v>
+        <v>37</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>63</v>
+        <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="3" t="s">
-        <v>80</v>
+        <v>41</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>64</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>67</v>
+        <v>28</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>66</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="3" t="s">
-        <v>81</v>
+        <v>42</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="3" t="s">
-        <v>82</v>
+        <v>43</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>71</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>72</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="3" t="s">
-        <v>73</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>74</v>
+        <v>35</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>62</v>
+        <v>23</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>75</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -997,7 +763,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE007A3-BDC4-4CCF-89DD-DFF030394921}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1014,15 +780,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>84</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="156.75" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>83</v>
+        <v>44</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>85</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1030,11 +796,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E22CFC9-75A9-4703-AAF7-30F647CF300B}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1052,316 +818,114 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>59</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BE905CA-1CE9-466F-88A4-C019229BCBBF}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="24.265625" customWidth="1"/>
-    <col min="3" max="3" width="20.265625" customWidth="1"/>
-    <col min="4" max="4" width="19.59765625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="2"/>
-    </row>
-    <row r="7" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="32.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>